<commit_message>
edits to validation files (username and password)
</commit_message>
<xml_diff>
--- a/Test Case.xlsx
+++ b/Test Case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_Shareon O'Brien\Documents\Vector Technology Institute\Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kraine\Documents\NetBeansProjects\VectorSoftwareEngineering20230515-develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4224D57F-1F4E-4B82-83FC-5E22037C7E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B7C306-8438-43AC-849B-596EA33EDEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{E5D638F0-F4DC-4CED-A8B3-F32EF72281E2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" activeTab="3" xr2:uid="{E5D638F0-F4DC-4CED-A8B3-F32EF72281E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Structure" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>1. Enter valid password 2. Re-enter password to confirm                              3. Click on login/register</t>
   </si>
   <si>
-    <t>Creation of a password that has: 1. Capitol letters    2. Characters &amp; symbol                     3. No space              4. Numbers</t>
-  </si>
-  <si>
     <t>TS_EFL_Password_003.2</t>
   </si>
   <si>
@@ -307,6 +304,14 @@
   </si>
   <si>
     <t>Prompt to create username that fufils all requirements</t>
+  </si>
+  <si>
+    <t>Creation of a password that has: 
+1. Capital letters 
+2. Characters &amp; symbol 
+3. No space 
+4. Numbers
+5. At least 8 characters</t>
   </si>
 </sst>
 </file>
@@ -713,52 +718,52 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -806,22 +811,22 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,7 +834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -837,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -845,22 +850,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -895,7 +900,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -924,7 +929,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="5" t="s">
         <v>21</v>
@@ -951,7 +956,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
@@ -977,7 +982,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1003,7 +1008,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
     </row>
   </sheetData>
@@ -1019,22 +1024,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1050,7 +1055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1058,22 +1063,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1113,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1137,7 +1142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="5" t="s">
         <v>45</v>
@@ -1164,7 +1169,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
@@ -1190,7 +1195,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>45</v>
       </c>
@@ -1216,7 +1221,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
@@ -1242,7 +1247,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>45</v>
       </c>
@@ -1268,7 +1273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
@@ -1303,26 +1308,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF654A1F-CC5E-431E-ACDE-2754610AEBB3}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.36328125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1338,7 +1343,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1346,22 +1351,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1396,7 +1401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>69</v>
       </c>
@@ -1416,7 +1421,7 @@
         <v>33</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>25</v>
@@ -1425,34 +1430,34 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="116" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1461,7 +1466,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1470,7 +1475,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
     </row>
   </sheetData>
@@ -1482,26 +1487,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65682CAD-DB0F-4B78-B008-EB2BB6EA3FDF}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B6" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1517,7 +1522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1525,22 +1530,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1575,27 +1580,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>25</v>
@@ -1604,32 +1609,32 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1638,7 +1643,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1647,7 +1652,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
     </row>
   </sheetData>

</xml_diff>